<commit_message>
Fix mistake in summary table
</commit_message>
<xml_diff>
--- a/Papers/InProgress/HajekAndersonControversy/Summary.xlsx
+++ b/Papers/InProgress/HajekAndersonControversy/Summary.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="6920" windowWidth="11680" windowHeight="8420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$14</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="37">
   <si>
     <t>Proof</t>
   </si>
@@ -63,9 +66,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>R (KB)</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>R (K4)</t>
-  </si>
-  <si>
-    <t>CS (S5)</t>
   </si>
   <si>
     <t>P (KB)</t>
@@ -705,8 +702,8 @@
   </sheetPr>
   <dimension ref="B1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -714,8 +711,7 @@
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
@@ -723,7 +719,7 @@
     <col min="12" max="12" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="16" thickBot="1"/>
@@ -732,22 +728,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>2</v>
@@ -776,43 +772,43 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="N3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:15">
@@ -820,43 +816,43 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -864,43 +860,43 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -908,221 +904,221 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="L7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:15">
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>13</v>
@@ -1133,33 +1129,33 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>13</v>
@@ -1168,42 +1164,42 @@
         <v>13</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>13</v>
@@ -1212,31 +1208,31 @@
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>